<commit_message>
Data Sample Folder moved to Database Folder
</commit_message>
<xml_diff>
--- a/Documentation/Delegation of Tasks.xlsx
+++ b/Documentation/Delegation of Tasks.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Softdev" sheetId="1" r:id="rId1"/>
     <sheet name="Quality" sheetId="2" r:id="rId2"/>
+    <sheet name="Projman" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>To do list</t>
   </si>
@@ -176,12 +178,30 @@
   <si>
     <t>Software Quality Assurance</t>
   </si>
+  <si>
+    <t>Data Query of other system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Kung yung Data ba na kailangan nila makita ay sa Monitoring System or sa System nila..?
+     - kasi pwede namin nilang tignan mismo yung data na kailangan nila sa monitoring system
+2) Kung yung requesting ba ay sa system namin or sa kanila
+     - </t>
+  </si>
+  <si>
+    <t>Aira Carpio</t>
+  </si>
+  <si>
+    <t>Gail Haboc</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +234,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,10 +259,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -243,20 +271,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +659,9 @@
       <c r="D3" s="5">
         <v>42808</v>
       </c>
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -618,9 +673,14 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>28</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -628,165 +688,230 @@
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="9">
+      <c r="C11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="8">
         <v>42808</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9">
+      <c r="C12" s="18"/>
+      <c r="D12" s="8">
         <v>42814</v>
       </c>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="8">
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" t="s">
+      <c r="D18" s="12">
+        <v>42808</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8" t="s">
+      <c r="D19" s="12">
+        <v>42808</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="C21" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="5">
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="5">
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="5">
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D27" s="9">
         <v>42805</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="D5:D9"/>
+    <mergeCell ref="E5:E9"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +949,231 @@
         <v>34</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>